<commit_message>
Cleaned up the figures.
</commit_message>
<xml_diff>
--- a/MANUSCRIPT/FIGURES/Table1.xlsx
+++ b/MANUSCRIPT/FIGURES/Table1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fsu-my.sharepoint.com/personal/meh03c_fsu_edu/Documents/MANUSCRIPTS/WORKING/covid-differential-privacy/MANUSCRIPT/FIGURES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50A005D4-A19A-48B8-9F77-B6F84087722D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{50A005D4-A19A-48B8-9F77-B6F84087722D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{611575DC-0A22-4182-8ADD-F5CCA8077AF2}"/>
   <bookViews>
-    <workbookView xWindow="7215" yWindow="1860" windowWidth="22470" windowHeight="14010" xr2:uid="{2B9BA370-26DC-47A0-B047-281044EDCD9C}"/>
+    <workbookView xWindow="8895" yWindow="1590" windowWidth="22470" windowHeight="14010" activeTab="1" xr2:uid="{2B9BA370-26DC-47A0-B047-281044EDCD9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>Pop. Size</t>
   </si>
@@ -78,6 +79,39 @@
   </si>
   <si>
     <t>&lt; 500K</t>
+  </si>
+  <si>
+    <t>Med. Abs. % Err</t>
+  </si>
+  <si>
+    <t>Mean Abs. % Err</t>
+  </si>
+  <si>
+    <t>% of county-age-sex groups</t>
+  </si>
+  <si>
+    <t>&lt; 1,000</t>
+  </si>
+  <si>
+    <t>&lt; 2,500</t>
+  </si>
+  <si>
+    <t>&lt; 5,000</t>
+  </si>
+  <si>
+    <t>&lt; 10,000</t>
+  </si>
+  <si>
+    <t>&lt; 20,000</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Age-Sex</t>
+  </si>
+  <si>
+    <t>Race/Ethnicity</t>
   </si>
 </sst>
 </file>
@@ -86,10 +120,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +157,28 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -144,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -161,15 +217,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -177,18 +242,42 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -507,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7D06C9-4819-4851-8E28-9C36EE52A743}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,6 +943,289 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9A89FC-9EA5-485B-A868-8A11E93863B6}">
+  <dimension ref="A3:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="D5" s="14">
+        <v>17950</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.42899999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="13">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="D6" s="14">
+        <v>28836</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="13">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C7" s="13">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="D7" s="14">
+        <v>34379</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.82199999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="13">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C8" s="13">
+        <v>0.216</v>
+      </c>
+      <c r="D8" s="14">
+        <v>37711</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.90200000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="C9" s="13">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="D9" s="14">
+        <v>39735</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="16">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="C10" s="16">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="D10" s="17">
+        <v>41812</v>
+      </c>
+      <c r="E10" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="13">
+        <v>0.1566265</v>
+      </c>
+      <c r="C13" s="13">
+        <v>0.47212500000000002</v>
+      </c>
+      <c r="D13" s="14">
+        <v>16085</v>
+      </c>
+      <c r="E13" s="13">
+        <v>0.60404100000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="13">
+        <v>0.1161972</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0.41463100000000003</v>
+      </c>
+      <c r="D14" s="14">
+        <v>18460</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0.69322899999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="13">
+        <v>9.4594600000000001E-2</v>
+      </c>
+      <c r="C15" s="13">
+        <v>0.379965</v>
+      </c>
+      <c r="D15" s="14">
+        <v>20202</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0.75864699999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="13">
+        <v>7.6631900000000003E-2</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0.35025699999999999</v>
+      </c>
+      <c r="D16" s="14">
+        <v>21950</v>
+      </c>
+      <c r="E16" s="13">
+        <v>0.82428900000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="13">
+        <v>6.2764500000000001E-2</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0.32695299999999999</v>
+      </c>
+      <c r="D17" s="14">
+        <v>23533</v>
+      </c>
+      <c r="E17" s="13">
+        <v>0.88373599999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="16">
+        <v>4.1666700000000001E-2</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0.28909099999999999</v>
+      </c>
+      <c r="D18" s="17">
+        <v>26629</v>
+      </c>
+      <c r="E18" s="16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A11:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1042,18 +1414,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1075,18 +1447,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EFCD92B-A32C-424B-8883-59CC924930E3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A46762F-9BF2-41F6-B272-4BC5D6202139}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EFCD92B-A32C-424B-8883-59CC924930E3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>